<commit_message>
Added ability to perform u-turns
</commit_message>
<xml_diff>
--- a/angle_calculator.xlsx
+++ b/angle_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zymi\Documents\GitHub\Magisterka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D008E58-3007-4849-9F9F-13B49D67C384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDC408-2D6C-42F3-BEEF-334240490F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="21600" xr2:uid="{DFFFD8FD-3FB1-4B76-9832-5FADB95B7C6A}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{DFFFD8FD-3FB1-4B76-9832-5FADB95B7C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -13280,8 +13280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647645AE-9AC7-4AE8-BB8B-339294A3ACA7}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14274,8 +14274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37067286-E7F8-4C0F-AB3B-2D7CCAFDC4B2}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>